<commit_message>
Fix bug with Adding customer not redisplaying screen. Put invoice formating and printing into a separate class. Fix a bunch of bugs with parameters.
</commit_message>
<xml_diff>
--- a/SampleCheckbook.xlsx
+++ b/SampleCheckbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Products\BusinessCheckBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E154254F-03D5-45F5-98A8-258A19AE8422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E756CE1D-BE9D-4175-8988-699303B5F705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChartOfAccounts" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="169">
   <si>
     <t>IsActive</t>
   </si>
@@ -870,13 +870,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1167,10 +1172,10 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
@@ -1184,13 +1189,13 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1201,9 +1206,12 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" t="s">
@@ -1218,10 +1226,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -1238,10 +1246,10 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -1258,10 +1266,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -1278,10 +1286,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -1298,10 +1306,10 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -1318,10 +1326,10 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
@@ -1338,16 +1346,13 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,10 +1363,10 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
         <v>41</v>
@@ -1375,10 +1380,13 @@
         <v>21</v>
       </c>
       <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
         <v>64</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
       </c>
       <c r="F28" t="s">
         <v>41</v>
@@ -1392,10 +1400,10 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>64</v>
@@ -1412,10 +1420,10 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
         <v>64</v>
@@ -1432,10 +1440,10 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
         <v>64</v>
@@ -1452,16 +1460,16 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
         <v>64</v>
       </c>
       <c r="F32" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1472,16 +1480,16 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,16 +1500,16 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,16 +1520,16 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
         <v>64</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,16 +1540,16 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
         <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,10 +1560,10 @@
         <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E37" t="s">
         <v>64</v>
@@ -1572,10 +1580,10 @@
         <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
         <v>64</v>
@@ -1592,16 +1600,16 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
         <v>64</v>
       </c>
       <c r="F39" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,16 +1620,16 @@
         <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>64</v>
       </c>
       <c r="F40" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1632,16 +1640,13 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1652,9 +1657,12 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
         <v>85</v>
       </c>
       <c r="F42" t="s">
@@ -1669,10 +1677,10 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
         <v>85</v>
@@ -1689,10 +1697,10 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
         <v>85</v>
@@ -1709,10 +1717,10 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D45" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
@@ -1729,10 +1737,10 @@
         <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
         <v>85</v>
@@ -1749,10 +1757,10 @@
         <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E47" t="s">
         <v>85</v>
@@ -1769,16 +1777,13 @@
         <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D48" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F48" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,13 +1794,13 @@
         <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F49" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1803,29 +1808,12 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2138,7 +2126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>